<commit_message>
Complete Serial Communication with mask
</commit_message>
<xml_diff>
--- a/Mask_proto/Termie/bin/Debug/default.xlsx
+++ b/Mask_proto/Termie/bin/Debug/default.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,324 +400,100 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>3.2060000896453857</v>
+        <v>6.2620000839233398</v>
       </c>
       <c r="B2">
-        <v>4.2013089114334434E-5</v>
+        <v>1.0779603876187593E-8</v>
       </c>
       <c r="C2">
-        <v>1.7566309543326497E-4</v>
+        <v>1.0561709132161923E-5</v>
       </c>
       <c r="D2">
-        <v>2.5348867449537238E-9</v>
+        <v>1.6614868945907801E-4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>3.437000036239624</v>
+        <v>6.435999870300293</v>
       </c>
       <c r="B3">
-        <v>1.708985073491931E-4</v>
+        <v>4.2252446291968226E-5</v>
       </c>
       <c r="C3">
-        <v>2.6950719433926906E-9</v>
+        <v>4.1256701166503262E-8</v>
       </c>
       <c r="D3">
-        <v>4.1199238465239318E-11</v>
+        <v>1.7660192679613829E-4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>3.6119999885559082</v>
+        <v>6.6449999809265137</v>
       </c>
       <c r="B4">
-        <v>2.6999157398677198E-6</v>
+        <v>6.6763055883711786E-7</v>
       </c>
       <c r="C4">
-        <v>1.0622477020660881E-5</v>
+        <v>4.3917654693359509E-5</v>
       </c>
       <c r="D4">
-        <v>1.6225830279381626E-7</v>
+        <v>1.0140003503522621E-8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>3.8090000152587891</v>
+        <v>6.8480000495910645</v>
       </c>
       <c r="B5">
-        <v>4.3201434891670942E-5</v>
+        <v>1.0431725705473127E-8</v>
       </c>
       <c r="C5">
-        <v>6.6764494022208964E-7</v>
+        <v>2.7598691758612404E-6</v>
       </c>
       <c r="D5">
-        <v>2.5349435883725846E-9</v>
+        <v>4.1532508475938812E-5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>4.0130000114440918</v>
+        <v>7.0510001182556152</v>
       </c>
       <c r="B6">
-        <v>1.0919807209575083E-5</v>
+        <v>2.6704638003138825E-6</v>
       </c>
       <c r="C6">
-        <v>1.0919806300080381E-5</v>
+        <v>1.7061100265891582E-7</v>
       </c>
       <c r="D6">
-        <v>6.3382127324373982E-10</v>
+        <v>2.5957833713619038E-6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>4.2170000076293945</v>
+        <v>7.2560000419616699</v>
       </c>
       <c r="B7">
-        <v>1.7249546147013461E-7</v>
+        <v>2.6224837856858585E-9</v>
       </c>
       <c r="C7">
-        <v>1.0682088031899184E-5</v>
+        <v>2.5785427126834293E-9</v>
       </c>
       <c r="D7">
-        <v>4.0977173043632575E-11</v>
+        <v>1.6225455112817144E-7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>4.4510002136230469</v>
+        <v>7.4559998512268066</v>
       </c>
       <c r="B8">
-        <v>4.2188023741118741E-8</v>
+        <v>6.899820732542139E-7</v>
       </c>
       <c r="C8">
-        <v>6.675868462480139E-7</v>
+        <v>1.031508034543549E-8</v>
       </c>
       <c r="D8">
-        <v>1.0383366316091269E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>4.6230001449584961</v>
-      </c>
-      <c r="B9">
-        <v>1.7063653956483904E-7</v>
-      </c>
-      <c r="C9">
-        <v>2.5931525815536816E-9</v>
-      </c>
-      <c r="D9">
-        <v>6.4898949858616106E-7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>4.8260002136230469</v>
-      </c>
-      <c r="B10">
-        <v>4.4160704419482499E-5</v>
-      </c>
-      <c r="C10">
-        <v>1.066478372280244E-8</v>
-      </c>
-      <c r="D10">
-        <v>4.0562728287341088E-8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>5.0390000343322754</v>
-      </c>
-      <c r="B11">
-        <v>6.8996774871266098E-7</v>
-      </c>
-      <c r="C11">
-        <v>1.6900601622182876E-4</v>
-      </c>
-      <c r="D11">
-        <v>2.5348876331321435E-9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>5.2329998016357422</v>
-      </c>
-      <c r="B12">
-        <v>1.7662801838014275E-4</v>
-      </c>
-      <c r="C12">
-        <v>1.0859735994017683E-5</v>
-      </c>
-      <c r="D12">
-        <v>6.4893134776866646E-7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>5.4739999771118164</v>
-      </c>
-      <c r="B13">
-        <v>1.6875567609986319E-7</v>
-      </c>
-      <c r="C13">
-        <v>2.5789412827492697E-9</v>
-      </c>
-      <c r="D13">
-        <v>4.3912055843975395E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>5.7309999465942383</v>
-      </c>
-      <c r="B14">
-        <v>1.1039245691790711E-5</v>
-      </c>
-      <c r="C14">
-        <v>1.6782792044978123E-7</v>
-      </c>
-      <c r="D14">
-        <v>1.6611888713669032E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>5.880000114440918</v>
-      </c>
-      <c r="B15">
-        <v>4.3202391680097207E-5</v>
-      </c>
-      <c r="C15">
-        <v>4.1022051533445847E-8</v>
-      </c>
-      <c r="D15">
-        <v>1.6225091314936435E-7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>16.781999588012695</v>
-      </c>
-      <c r="B16">
-        <v>1.1040180652344134E-5</v>
-      </c>
-      <c r="C16">
-        <v>1.6595447505096672E-7</v>
-      </c>
-      <c r="D16">
-        <v>1.0382897926319856E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>17.031999588012695</v>
-      </c>
-      <c r="B17">
-        <v>4.2488973122090101E-5</v>
-      </c>
-      <c r="C17">
-        <v>4.2191647509071117E-8</v>
-      </c>
-      <c r="D17">
-        <v>6.4893117723840987E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>17.281999588012695</v>
-      </c>
-      <c r="B18">
-        <v>1.7661310266703367E-4</v>
-      </c>
-      <c r="C18">
-        <v>6.7134095615983824E-7</v>
-      </c>
-      <c r="D18">
-        <v>6.4894544493654394E-7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>17.461999893188477</v>
-      </c>
-      <c r="B19">
-        <v>6.5646923985696048E-7</v>
-      </c>
-      <c r="C19">
-        <v>1.0489705104532732E-8</v>
-      </c>
-      <c r="D19">
-        <v>1.0978013960993849E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>17.635000228881836</v>
-      </c>
-      <c r="B20">
-        <v>1.0663193883431177E-8</v>
-      </c>
-      <c r="C20">
-        <v>1.7089470929931849E-4</v>
-      </c>
-      <c r="D20">
-        <v>6.4898955542957992E-7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>17.809000015258789</v>
-      </c>
-      <c r="B21">
-        <v>1.7089105676859617E-4</v>
-      </c>
-      <c r="C21">
-        <v>1.0315305054575674E-8</v>
-      </c>
-      <c r="D21">
-        <v>1.6225457954988087E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>18.023000717163086</v>
-      </c>
-      <c r="B22">
-        <v>4.415791408973746E-5</v>
-      </c>
-      <c r="C22">
-        <v>4.4158841774333268E-5</v>
-      </c>
-      <c r="D22">
-        <v>4.0561840108921388E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>18.23699951171875</v>
-      </c>
-      <c r="B23">
-        <v>1.0561249837337527E-5</v>
-      </c>
-      <c r="C23">
-        <v>1.7565938469488174E-4</v>
-      </c>
-      <c r="D23">
-        <v>1.6222551835198828E-7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>18.438999176025391</v>
-      </c>
-      <c r="B24">
-        <v>4.2425376989285724E-8</v>
-      </c>
-      <c r="C24">
-        <v>4.3439860746730119E-5</v>
-      </c>
-      <c r="D24">
-        <v>1.0140227324484385E-8</v>
+        <v>1.661524293012917E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>